<commit_message>
Cambios en algunos nombres y descripciones
Cambios en algunos nombres y descripciones
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion09/ESCALETA_FINAL_CN_11_09_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion09/ESCALETA_FINAL_CN_11_09_CO.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="235">
   <si>
     <t>Asignatura</t>
   </si>
@@ -525,90 +525,6 @@
     <t>Actividad para practicar el cálculo del pH de disoluciones ácidas y básicas</t>
   </si>
   <si>
-    <r>
-      <t>Calcula el pH o la concentración de iones H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">+ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> en disoluciones </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Actividad para practicar el cálculo del pH y  concentración de iones H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para clasificar ácidos y bases fuertes y débiles </t>
   </si>
   <si>
@@ -663,9 +579,6 @@
     <t>Recurso M11A-01</t>
   </si>
   <si>
-    <t>Actividad que permite identificar los conceptos importantes en las celdas electroquímicas</t>
-  </si>
-  <si>
     <t>Interactivo con animación que muestra la electrólisis y sus aplicaciones industriales</t>
   </si>
   <si>
@@ -678,9 +591,6 @@
     <t>Recurso M101A-05</t>
   </si>
   <si>
-    <t>Actividad que propone realizar un experimento para determinar la concentración de una disolución mediante una valoración ácido-base</t>
-  </si>
-  <si>
     <t>Actividad con animación incluida para practicar las diferencias entre los ácidos y las bases</t>
   </si>
   <si>
@@ -735,9 +645,6 @@
     <t>Competencias: cantidad de hidrogenocarbonato en un antiácido</t>
   </si>
   <si>
-    <t>La autodisociación del agua</t>
-  </si>
-  <si>
     <t>Secuencia de imágenes que permite explicar la propiedad del agua de actuar como ácido o base</t>
   </si>
   <si>
@@ -753,12 +660,6 @@
     <t>RM_01_02_CO</t>
   </si>
   <si>
-    <t xml:space="preserve">La medida de la acidez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactivo para explicar el concepto de pH y pOH en disoluciones </t>
-  </si>
-  <si>
     <t>Recurso F6-02</t>
   </si>
   <si>
@@ -811,13 +712,37 @@
   </si>
   <si>
     <t>Aplicaciones de la celdas galvánicas en la vida diaria</t>
+  </si>
+  <si>
+    <t>El equilibrio iónico del agua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El pH y la fuerza de los ácidos y las bases </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite explicar el pH en las disoluciones acuosas y la fuerza relativa de ácidos y bases </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realiza los cálculos de las disoluciones </t>
+  </si>
+  <si>
+    <t>Actividad para practicar los cálculos de pH, pOH  y  las concentraciones de iones hidronio e hidroxilo</t>
+  </si>
+  <si>
+    <t>Actividades sobre Los indicadores ácido-base</t>
+  </si>
+  <si>
+    <t>Actividad que permite afianzar algunos conceptos importantes en las celdas electroquímicas</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar una práctica de laboratorio para determinar la concentración de una disolución mediante una valoración ácido-base</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,22 +769,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1521,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="G28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,7 +1826,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="21" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="H8" s="22">
         <v>3</v>
@@ -1926,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="K8" s="24" t="s">
         <v>69</v>
@@ -1935,7 +1844,7 @@
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
       <c r="O8" s="27" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="P8" s="26" t="s">
         <v>19</v>
@@ -1947,13 +1856,13 @@
         <v>150</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
@@ -2117,7 +2026,7 @@
         <v>151</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>152</v>
@@ -2139,7 +2048,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="21" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="H12" s="22">
         <v>5</v>
@@ -2148,7 +2057,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>69</v>
@@ -2172,7 +2081,7 @@
         <v>156</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>158</v>
@@ -2334,13 +2243,13 @@
         <v>19</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>132</v>
@@ -2349,7 +2258,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>67</v>
       </c>
@@ -2369,7 +2278,7 @@
         <v>121</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="H16" s="22">
         <v>7</v>
@@ -2378,7 +2287,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>165</v>
+        <v>231</v>
       </c>
       <c r="K16" s="24" t="s">
         <v>69</v>
@@ -2404,7 +2313,7 @@
         <v>151</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>152</v>
@@ -2439,7 +2348,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K17" s="24" t="s">
         <v>70</v>
@@ -2454,13 +2363,13 @@
         <v>19</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>135</v>
@@ -2498,7 +2407,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K18" s="24" t="s">
         <v>70</v>
@@ -2513,16 +2422,16 @@
         <v>19</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>162</v>
@@ -2557,7 +2466,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K19" s="24" t="s">
         <v>70</v>
@@ -2572,16 +2481,16 @@
         <v>19</v>
       </c>
       <c r="Q19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="T19" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="R19" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>162</v>
@@ -2647,7 +2556,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K21" s="24" t="s">
         <v>69</v>
@@ -2673,7 +2582,7 @@
         <v>151</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="U21" s="2" t="s">
         <v>152</v>
@@ -2695,7 +2604,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H22" s="22">
         <v>12</v>
@@ -2704,7 +2613,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="K22" s="24" t="s">
         <v>69</v>
@@ -2730,7 +2639,7 @@
         <v>156</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>158</v>
@@ -2809,7 +2718,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>138</v>
+        <v>232</v>
       </c>
       <c r="K23" s="24" t="s">
         <v>70</v>
@@ -2826,13 +2735,13 @@
         <v>19</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T23" s="11" t="s">
         <v>138</v>
@@ -2967,7 +2876,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K27" s="24" t="s">
         <v>70</v>
@@ -2976,19 +2885,19 @@
       <c r="M27" s="28"/>
       <c r="N27" s="28"/>
       <c r="O27" s="27" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="P27" s="26" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S27" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T27" s="11" t="s">
         <v>139</v>
@@ -3024,7 +2933,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K28" s="24" t="s">
         <v>70</v>
@@ -3039,16 +2948,16 @@
         <v>19</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R28" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="S28" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="T28" s="11" t="s">
         <v>194</v>
-      </c>
-      <c r="S28" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="T28" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="U28" s="2" t="s">
         <v>162</v>
@@ -3081,7 +2990,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K29" s="24" t="s">
         <v>70</v>
@@ -3096,16 +3005,16 @@
         <v>19</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S29" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="T29" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="T29" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>162</v>
@@ -3278,7 +3187,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K34" s="24" t="s">
         <v>69</v>
@@ -3304,7 +3213,7 @@
         <v>151</v>
       </c>
       <c r="T34" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>152</v>
@@ -3326,7 +3235,7 @@
       <c r="E35" s="19"/>
       <c r="F35" s="20"/>
       <c r="G35" s="21" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H35" s="22">
         <v>18</v>
@@ -3335,7 +3244,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="K35" s="24" t="s">
         <v>69</v>
@@ -3361,7 +3270,7 @@
         <v>156</v>
       </c>
       <c r="T35" s="11" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>158</v>
@@ -3438,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K36" s="24" t="s">
         <v>70</v>
@@ -3453,13 +3362,13 @@
         <v>19</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S36" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T36" s="11" t="s">
         <v>142</v>
@@ -3493,7 +3402,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K37" s="24" t="s">
         <v>70</v>
@@ -3508,13 +3417,13 @@
         <v>19</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R37" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S37" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T37" s="11" t="s">
         <v>143</v>
@@ -3550,7 +3459,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K38" s="24" t="s">
         <v>70</v>
@@ -3565,13 +3474,13 @@
         <v>19</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R38" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S38" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T38" s="11" t="s">
         <v>144</v>
@@ -3660,7 +3569,7 @@
         <v>98</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="21"/>
@@ -3759,7 +3668,7 @@
         <v>98</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>127</v>
@@ -3831,7 +3740,7 @@
         <v>129</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H46" s="22">
         <v>22</v>
@@ -3840,7 +3749,7 @@
         <v>19</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K46" s="24" t="s">
         <v>69</v>
@@ -3851,7 +3760,7 @@
       <c r="M46" s="28"/>
       <c r="N46" s="28"/>
       <c r="O46" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="P46" s="26" t="s">
         <v>19</v>
@@ -3863,13 +3772,13 @@
         <v>155</v>
       </c>
       <c r="S46" s="11" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:67" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3899,7 +3808,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K47" s="24" t="s">
         <v>70</v>
@@ -3916,16 +3825,16 @@
         <v>19</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R47" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S47" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T47" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>162</v>
@@ -3995,7 +3904,7 @@
         <v>129</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H48" s="22">
         <v>24</v>
@@ -4004,7 +3913,7 @@
         <v>20</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="K48" s="24" t="s">
         <v>69</v>
@@ -4030,7 +3939,7 @@
         <v>151</v>
       </c>
       <c r="T48" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="U48" s="2" t="s">
         <v>152</v>
@@ -4107,7 +4016,7 @@
         <v>20</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K49" s="24" t="s">
         <v>70</v>
@@ -4122,13 +4031,13 @@
         <v>20</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R49" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T49" s="11" t="s">
         <v>133</v>
@@ -4164,7 +4073,7 @@
         <v>20</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K50" s="24" t="s">
         <v>69</v>
@@ -4190,7 +4099,7 @@
         <v>151</v>
       </c>
       <c r="T50" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>152</v>
@@ -4207,7 +4116,7 @@
         <v>91</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E51" s="19"/>
       <c r="F51" s="20"/>
@@ -4221,7 +4130,7 @@
         <v>20</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="K51" s="24" t="s">
         <v>70</v>
@@ -4238,16 +4147,16 @@
         <v>19</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="R51" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="U51" s="2" t="s">
         <v>162</v>
@@ -4264,12 +4173,12 @@
         <v>91</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E52" s="19"/>
       <c r="F52" s="20"/>
       <c r="G52" s="21" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H52" s="22">
         <v>28</v>
@@ -4278,7 +4187,7 @@
         <v>20</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K52" s="24" t="s">
         <v>70</v>
@@ -4295,16 +4204,16 @@
         <v>19</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="R52" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="T52" s="11" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>162</v>
@@ -4381,7 +4290,7 @@
         <v>20</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K53" s="24" t="s">
         <v>69</v>
@@ -4426,7 +4335,7 @@
         <v>20</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="K54" s="24" t="s">
         <v>69</v>
@@ -4452,7 +4361,7 @@
         <v>151</v>
       </c>
       <c r="T54" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U54" s="2" t="s">
         <v>152</v>
@@ -4472,7 +4381,7 @@
       <c r="E55" s="19"/>
       <c r="F55" s="20"/>
       <c r="G55" s="21" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H55" s="22">
         <v>31</v>
@@ -4481,7 +4390,7 @@
         <v>20</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K55" s="24" t="s">
         <v>69</v>
@@ -4507,7 +4416,7 @@
         <v>151</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="U55" s="2" t="s">
         <v>152</v>
@@ -5527,6 +5436,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -5542,11 +5456,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>